<commit_message>
Added Pinout & Updated BOM
</commit_message>
<xml_diff>
--- a/Pick Place for MiniESP32_Panel_BOM.xlsx
+++ b/Pick Place for MiniESP32_Panel_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_DATEN\Alexander\Projekte\_Projektordner\MiniESP32\Altium\Outputs\Fertigung\V1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDB7349-D34B-455D-BB9F-43B73A6A3CD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9453D19-9D63-4572-B2FB-15EF27FF3C60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DDC982FF-94B5-4844-B014-1947C088C29E}"/>
+    <workbookView xWindow="38280" yWindow="5985" windowWidth="19440" windowHeight="15600" xr2:uid="{DDC982FF-94B5-4844-B014-1947C088C29E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle3" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="141">
   <si>
     <t>Designator</t>
   </si>
@@ -438,6 +438,27 @@
   </si>
   <si>
     <t>C20917</t>
+  </si>
+  <si>
+    <t>C22843</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>C118141</t>
+  </si>
+  <si>
+    <t>C7464026</t>
+  </si>
+  <si>
+    <t>JLCPCB Part #</t>
+  </si>
+  <si>
+    <t>C14663</t>
+  </si>
+  <si>
+    <t>C96446</t>
   </si>
 </sst>
 </file>
@@ -453,12 +474,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -473,8 +500,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -789,326 +817,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1326BD3-2EEE-4807-94A7-D047B700C715}">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83:D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D21" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D23" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D25" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="D26" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="D27" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1118,8 +1230,11 @@
       <c r="C29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1129,8 +1244,11 @@
       <c r="C30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1140,8 +1258,11 @@
       <c r="C31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1151,8 +1272,11 @@
       <c r="C32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1162,8 +1286,11 @@
       <c r="C33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1173,8 +1300,11 @@
       <c r="C34" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -1184,8 +1314,11 @@
       <c r="C35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -1195,8 +1328,11 @@
       <c r="C36" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -1206,8 +1342,11 @@
       <c r="C37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -1217,8 +1356,11 @@
       <c r="C38" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -1228,8 +1370,11 @@
       <c r="C39" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -1239,8 +1384,11 @@
       <c r="C40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -1250,8 +1398,11 @@
       <c r="C41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -1261,8 +1412,11 @@
       <c r="C42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -1272,8 +1426,11 @@
       <c r="C43" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -1283,8 +1440,11 @@
       <c r="C44" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -1294,8 +1454,9 @@
       <c r="C45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -1305,8 +1466,11 @@
       <c r="C46" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1316,8 +1480,11 @@
       <c r="C47" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -1327,8 +1494,11 @@
       <c r="C48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -1338,8 +1508,11 @@
       <c r="C49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -1349,8 +1522,11 @@
       <c r="C50" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>69</v>
       </c>
@@ -1360,8 +1536,11 @@
       <c r="C51" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -1371,8 +1550,11 @@
       <c r="C52" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>71</v>
       </c>
@@ -1382,8 +1564,11 @@
       <c r="C53" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -1393,8 +1578,11 @@
       <c r="C54" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>73</v>
       </c>
@@ -1404,8 +1592,11 @@
       <c r="C55" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -1415,8 +1606,11 @@
       <c r="C56" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -1426,8 +1620,11 @@
       <c r="C57" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -1437,8 +1634,11 @@
       <c r="C58" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -1448,8 +1648,11 @@
       <c r="C59" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -1459,8 +1662,11 @@
       <c r="C60" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -1470,8 +1676,11 @@
       <c r="C61" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -1481,8 +1690,11 @@
       <c r="C62" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -1492,8 +1704,11 @@
       <c r="C63" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -1503,8 +1718,11 @@
       <c r="C64" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>83</v>
       </c>
@@ -1514,8 +1732,11 @@
       <c r="C65" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -1525,8 +1746,11 @@
       <c r="C66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -1536,8 +1760,11 @@
       <c r="C67" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -1547,8 +1774,11 @@
       <c r="C68" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -1558,8 +1788,11 @@
       <c r="C69" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -1569,8 +1802,11 @@
       <c r="C70" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -1580,8 +1816,11 @@
       <c r="C71" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -1591,8 +1830,9 @@
       <c r="C72" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -1602,8 +1842,11 @@
       <c r="C73" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>92</v>
       </c>
@@ -1613,8 +1856,11 @@
       <c r="C74" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>93</v>
       </c>
@@ -1624,8 +1870,11 @@
       <c r="C75" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>94</v>
       </c>
@@ -1635,8 +1884,11 @@
       <c r="C76" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>95</v>
       </c>
@@ -1646,8 +1898,11 @@
       <c r="C77" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>96</v>
       </c>
@@ -1657,8 +1912,11 @@
       <c r="C78" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>97</v>
       </c>
@@ -1668,8 +1926,11 @@
       <c r="C79" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>98</v>
       </c>
@@ -1679,8 +1940,11 @@
       <c r="C80" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>99</v>
       </c>
@@ -1690,8 +1954,11 @@
       <c r="C81" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>100</v>
       </c>
@@ -1701,8 +1968,11 @@
       <c r="C82" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>101</v>
       </c>
@@ -1712,8 +1982,11 @@
       <c r="C83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>102</v>
       </c>
@@ -1723,8 +1996,11 @@
       <c r="C84" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>103</v>
       </c>
@@ -1734,8 +2010,11 @@
       <c r="C85" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>104</v>
       </c>
@@ -1745,8 +2024,11 @@
       <c r="C86" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>105</v>
       </c>
@@ -1756,8 +2038,11 @@
       <c r="C87" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>106</v>
       </c>
@@ -1767,8 +2052,11 @@
       <c r="C88" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>107</v>
       </c>
@@ -1778,8 +2066,11 @@
       <c r="C89" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>108</v>
       </c>
@@ -1789,8 +2080,11 @@
       <c r="C90" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>109</v>
       </c>
@@ -1800,8 +2094,11 @@
       <c r="C91" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>110</v>
       </c>
@@ -1811,8 +2108,11 @@
       <c r="C92" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>111</v>
       </c>
@@ -1822,8 +2122,11 @@
       <c r="C93" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>112</v>
       </c>
@@ -1833,8 +2136,11 @@
       <c r="C94" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>113</v>
       </c>
@@ -1844,8 +2150,11 @@
       <c r="C95" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>114</v>
       </c>
@@ -1855,8 +2164,11 @@
       <c r="C96" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>115</v>
       </c>
@@ -1866,8 +2178,11 @@
       <c r="C97" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>116</v>
       </c>
@@ -1877,8 +2192,11 @@
       <c r="C98" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>117</v>
       </c>
@@ -1888,8 +2206,9 @@
       <c r="C99" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>118</v>
       </c>
@@ -1899,8 +2218,11 @@
       <c r="C100" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>119</v>
       </c>
@@ -1910,8 +2232,11 @@
       <c r="C101" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>120</v>
       </c>
@@ -1921,8 +2246,11 @@
       <c r="C102" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>121</v>
       </c>
@@ -1932,8 +2260,11 @@
       <c r="C103" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>122</v>
       </c>
@@ -1943,8 +2274,11 @@
       <c r="C104" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>123</v>
       </c>
@@ -1954,8 +2288,11 @@
       <c r="C105" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>124</v>
       </c>
@@ -1965,8 +2302,11 @@
       <c r="C106" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>125</v>
       </c>
@@ -1976,8 +2316,11 @@
       <c r="C107" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>126</v>
       </c>
@@ -1987,8 +2330,11 @@
       <c r="C108" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>127</v>
       </c>
@@ -1996,6 +2342,9 @@
         <v>18</v>
       </c>
       <c r="C109" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>